<commit_message>
Aggiornamento dettaglio "gestione errore"
Aggiornamento del report checklist con dettaglio su "gestione errore" come richiesto da comunicazione del Team FSE
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SINCONXX/SINCON_S.R.L/GIAVA/6/report-checklist.xlsx
+++ b/GATEWAY/A1#111SINCONXX/SINCON_S.R.L/GIAVA/6/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGETTI\fse\testcase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lavoro\GIAVA\documentazione\FSE\Accreditamento\CERTIFICATO VACC - Casi di Test XML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A68F90-225C-4275-AC57-C96995E21527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9AC9890-260E-43EA-A71C-2D2207C7AA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="300">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1052,9 +1052,6 @@
     <t>2023-06-27T12:41:29+00:00</t>
   </si>
   <si>
-    <t>Nessuna in questo caso, nel flusso reale non può accadere che il token sia errato</t>
-  </si>
-  <si>
     <t>2023-06-27T13:19:14+00:00</t>
   </si>
   <si>
@@ -1064,9 +1061,6 @@
     <t>2.16.840.1.113883.2.9.2.160.4.4.b05e244762b1e472be89a93800cc3ee326743cecb55984bf12813addb8de66d0.8926cfb6f5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Errore simulato, impossibile che avvenga nella realtà</t>
-  </si>
-  <si>
     <t>2023-06-27T13:19:13+00:00</t>
   </si>
   <si>
@@ -1269,6 +1263,60 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.160.4.4.b05e244762b1e472be89a93800cc3ee326743cecb55984bf12813addb8de66d0.6e6c6d8ca5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione del campo "purpose_of_use")</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione del campo "action_id" del token)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione del confidentialityCode)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione del codice fiscale dell'assistito)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione del comune di residenza)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione del nome dell'assistito)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione del sesso dell'assistito)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione del campo section/text della request)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione del campo effectiveTime della request)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione dei dati relativi al vaccino somministrato)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione corretta della codifica della malattia per la quale si somministra la vaccinazione)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione del campo "action_id")</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione del campo "confidentialityCode")</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la corretta valorizzazione del codice fiscale dell'assistito)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione del comune di residenza dell'assistito)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione del cognome dell'assistito)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazione della sezione narrativa della request)</t>
+  </si>
+  <si>
+    <t>Al Medico viene segnalato un errore  nella validazione e si richiede all'utente di riprovare in un successivo momento. E' presente nell'applicativo una  "cruscotto" che permette di reinviare le eventuali validazioni fallite. L'operatore di backoffice visualizza le informazioni relative alla tipologia di errore che ha generato il fallimento della validazione ed attua le opportune modifiche per consentire la ritrasmissione del documento al GATEWAY (nel caso specifico la valorizzazionedei dati di esonero/omissione o differimento della somministrazione)</t>
   </si>
 </sst>
 </file>
@@ -4192,10 +4240,10 @@
   <dimension ref="A1:T670"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H59" sqref="H59"/>
+      <selection pane="bottomRight" activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4239,7 +4287,7 @@
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="41" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D2" s="40"/>
       <c r="F2" s="12"/>
@@ -4469,13 +4517,13 @@
         <v>45111</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>80</v>
@@ -4513,13 +4561,13 @@
         <v>45111</v>
       </c>
       <c r="G11" s="33" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H11" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="I11" s="24" t="s">
         <v>275</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>277</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>80</v>
@@ -4557,13 +4605,13 @@
         <v>45111</v>
       </c>
       <c r="G12" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="I12" s="24" t="s">
         <v>278</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>279</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>280</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>80</v>
@@ -4601,13 +4649,13 @@
         <v>45111</v>
       </c>
       <c r="G13" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="I13" s="24" t="s">
         <v>281</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>282</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>283</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>80</v>
@@ -4797,10 +4845,10 @@
         <v>45104</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I18" s="24" t="s">
         <v>204</v>
@@ -4813,14 +4861,14 @@
         <v>80</v>
       </c>
       <c r="M18" s="34" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N18" s="25"/>
       <c r="O18" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P18" s="25" t="s">
-        <v>211</v>
+        <v>282</v>
       </c>
       <c r="Q18" s="25"/>
       <c r="R18" s="26"/>
@@ -4865,14 +4913,14 @@
         <v>80</v>
       </c>
       <c r="M19" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N19" s="25"/>
       <c r="O19" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="P19" s="34" t="s">
-        <v>211</v>
+      <c r="P19" s="25" t="s">
+        <v>282</v>
       </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="26"/>
@@ -4901,10 +4949,10 @@
         <v>45104</v>
       </c>
       <c r="G20" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H20" s="36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I20" s="24" t="s">
         <v>204</v>
@@ -4917,14 +4965,14 @@
         <v>80</v>
       </c>
       <c r="M20" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N20" s="25"/>
       <c r="O20" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="P20" s="34" t="s">
-        <v>211</v>
+      <c r="P20" s="25" t="s">
+        <v>283</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
@@ -4969,14 +5017,14 @@
         <v>80</v>
       </c>
       <c r="M21" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N21" s="25"/>
       <c r="O21" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="P21" s="34" t="s">
-        <v>211</v>
+      <c r="P21" s="25" t="s">
+        <v>293</v>
       </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="26"/>
@@ -5105,13 +5153,13 @@
         <v>45105</v>
       </c>
       <c r="G24" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="I24" s="24" t="s">
         <v>237</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>238</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>239</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>80</v>
@@ -5121,14 +5169,14 @@
         <v>80</v>
       </c>
       <c r="M24" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N24" s="25"/>
       <c r="O24" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P24" s="25" t="s">
-        <v>211</v>
+        <v>284</v>
       </c>
       <c r="Q24" s="25"/>
       <c r="R24" s="26"/>
@@ -5157,13 +5205,13 @@
         <v>45105</v>
       </c>
       <c r="G25" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="I25" s="24" t="s">
         <v>240</v>
-      </c>
-      <c r="H25" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="I25" s="24" t="s">
-        <v>242</v>
       </c>
       <c r="J25" s="25" t="s">
         <v>80</v>
@@ -5173,14 +5221,14 @@
         <v>80</v>
       </c>
       <c r="M25" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N25" s="25"/>
       <c r="O25" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P25" s="25" t="s">
-        <v>211</v>
+        <v>285</v>
       </c>
       <c r="Q25" s="25"/>
       <c r="R25" s="26"/>
@@ -5209,13 +5257,13 @@
         <v>45105</v>
       </c>
       <c r="G26" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="H26" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="I26" s="24" t="s">
         <v>243</v>
-      </c>
-      <c r="H26" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="I26" s="24" t="s">
-        <v>245</v>
       </c>
       <c r="J26" s="25" t="s">
         <v>80</v>
@@ -5225,14 +5273,14 @@
         <v>80</v>
       </c>
       <c r="M26" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N26" s="25"/>
       <c r="O26" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P26" s="25" t="s">
-        <v>211</v>
+        <v>284</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="26"/>
@@ -5261,13 +5309,13 @@
         <v>45105</v>
       </c>
       <c r="G27" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="I27" s="24" t="s">
         <v>246</v>
-      </c>
-      <c r="H27" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="I27" s="24" t="s">
-        <v>248</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>80</v>
@@ -5277,14 +5325,14 @@
         <v>80</v>
       </c>
       <c r="M27" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N27" s="25"/>
       <c r="O27" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P27" s="25" t="s">
-        <v>211</v>
+        <v>286</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="26"/>
@@ -5313,13 +5361,13 @@
         <v>45105</v>
       </c>
       <c r="G28" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="I28" s="24" t="s">
         <v>249</v>
-      </c>
-      <c r="H28" s="24" t="s">
-        <v>250</v>
-      </c>
-      <c r="I28" s="24" t="s">
-        <v>251</v>
       </c>
       <c r="J28" s="25" t="s">
         <v>80</v>
@@ -5329,14 +5377,14 @@
         <v>80</v>
       </c>
       <c r="M28" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N28" s="25"/>
       <c r="O28" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P28" s="25" t="s">
-        <v>211</v>
+        <v>287</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="26"/>
@@ -5365,13 +5413,13 @@
         <v>45105</v>
       </c>
       <c r="G29" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="I29" s="24" t="s">
         <v>252</v>
-      </c>
-      <c r="H29" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>254</v>
       </c>
       <c r="J29" s="25" t="s">
         <v>80</v>
@@ -5381,14 +5429,14 @@
         <v>80</v>
       </c>
       <c r="M29" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N29" s="25"/>
       <c r="O29" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P29" s="25" t="s">
-        <v>211</v>
+        <v>288</v>
       </c>
       <c r="Q29" s="25"/>
       <c r="R29" s="26"/>
@@ -5417,13 +5465,13 @@
         <v>45105</v>
       </c>
       <c r="G30" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="H30" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="I30" s="24" t="s">
         <v>255</v>
-      </c>
-      <c r="H30" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="I30" s="24" t="s">
-        <v>257</v>
       </c>
       <c r="J30" s="25" t="s">
         <v>80</v>
@@ -5433,14 +5481,14 @@
         <v>80</v>
       </c>
       <c r="M30" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N30" s="25"/>
       <c r="O30" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P30" s="25" t="s">
-        <v>211</v>
+        <v>289</v>
       </c>
       <c r="Q30" s="25"/>
       <c r="R30" s="26"/>
@@ -5469,13 +5517,13 @@
         <v>45105</v>
       </c>
       <c r="G31" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="H31" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="I31" s="24" t="s">
         <v>258</v>
-      </c>
-      <c r="H31" s="24" t="s">
-        <v>259</v>
-      </c>
-      <c r="I31" s="24" t="s">
-        <v>260</v>
       </c>
       <c r="J31" s="25" t="s">
         <v>80</v>
@@ -5485,14 +5533,14 @@
         <v>80</v>
       </c>
       <c r="M31" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N31" s="25"/>
       <c r="O31" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P31" s="25" t="s">
-        <v>211</v>
+        <v>290</v>
       </c>
       <c r="Q31" s="25"/>
       <c r="R31" s="26"/>
@@ -5521,13 +5569,13 @@
         <v>45105</v>
       </c>
       <c r="G32" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="H32" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="I32" s="24" t="s">
         <v>261</v>
-      </c>
-      <c r="H32" s="24" t="s">
-        <v>262</v>
-      </c>
-      <c r="I32" s="24" t="s">
-        <v>263</v>
       </c>
       <c r="J32" s="25" t="s">
         <v>80</v>
@@ -5537,14 +5585,14 @@
         <v>80</v>
       </c>
       <c r="M32" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N32" s="25"/>
       <c r="O32" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P32" s="25" t="s">
-        <v>211</v>
+        <v>291</v>
       </c>
       <c r="Q32" s="25"/>
       <c r="R32" s="26"/>
@@ -5577,7 +5625,7 @@
         <v>196</v>
       </c>
       <c r="K33" s="25" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L33" s="25"/>
       <c r="M33" s="25"/>
@@ -5611,13 +5659,13 @@
         <v>45105</v>
       </c>
       <c r="G34" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="I34" s="24" t="s">
         <v>264</v>
-      </c>
-      <c r="H34" s="24" t="s">
-        <v>265</v>
-      </c>
-      <c r="I34" s="24" t="s">
-        <v>266</v>
       </c>
       <c r="J34" s="25" t="s">
         <v>80</v>
@@ -5627,14 +5675,14 @@
         <v>80</v>
       </c>
       <c r="M34" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N34" s="25"/>
       <c r="O34" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P34" s="25" t="s">
-        <v>211</v>
+        <v>292</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="26"/>
@@ -5667,7 +5715,7 @@
         <v>196</v>
       </c>
       <c r="K35" s="25" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L35" s="25"/>
       <c r="M35" s="25"/>
@@ -5701,13 +5749,13 @@
         <v>45105</v>
       </c>
       <c r="G36" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="H36" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="I36" s="24" t="s">
         <v>267</v>
-      </c>
-      <c r="H36" s="24" t="s">
-        <v>268</v>
-      </c>
-      <c r="I36" s="24" t="s">
-        <v>269</v>
       </c>
       <c r="J36" s="25" t="s">
         <v>80</v>
@@ -5717,14 +5765,14 @@
         <v>80</v>
       </c>
       <c r="M36" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N36" s="25"/>
       <c r="O36" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P36" s="25" t="s">
-        <v>211</v>
+        <v>299</v>
       </c>
       <c r="Q36" s="25"/>
       <c r="R36" s="26"/>
@@ -5753,13 +5801,13 @@
         <v>45104</v>
       </c>
       <c r="G37" s="33" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>80</v>
@@ -5769,14 +5817,14 @@
         <v>80</v>
       </c>
       <c r="M37" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N37" s="25"/>
       <c r="O37" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="P37" s="34" t="s">
-        <v>215</v>
+      <c r="P37" s="25" t="s">
+        <v>294</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="26"/>
@@ -5805,13 +5853,13 @@
         <v>45104</v>
       </c>
       <c r="G38" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="H38" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="I38" s="24" t="s">
         <v>219</v>
-      </c>
-      <c r="H38" s="24" t="s">
-        <v>220</v>
-      </c>
-      <c r="I38" s="24" t="s">
-        <v>221</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>80</v>
@@ -5821,14 +5869,14 @@
         <v>80</v>
       </c>
       <c r="M38" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N38" s="25"/>
       <c r="O38" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="P38" s="34" t="s">
-        <v>215</v>
+      <c r="P38" s="25" t="s">
+        <v>295</v>
       </c>
       <c r="Q38" s="25"/>
       <c r="R38" s="26"/>
@@ -5895,13 +5943,13 @@
         <v>45104</v>
       </c>
       <c r="G40" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="H40" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="I40" s="24" t="s">
         <v>216</v>
-      </c>
-      <c r="H40" s="24" t="s">
-        <v>217</v>
-      </c>
-      <c r="I40" s="24" t="s">
-        <v>218</v>
       </c>
       <c r="J40" s="25" t="s">
         <v>80</v>
@@ -5911,14 +5959,14 @@
         <v>80</v>
       </c>
       <c r="M40" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N40" s="25"/>
       <c r="O40" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="P40" s="34" t="s">
-        <v>215</v>
+      <c r="P40" s="25" t="s">
+        <v>296</v>
       </c>
       <c r="Q40" s="25"/>
       <c r="R40" s="26"/>
@@ -5947,13 +5995,13 @@
         <v>45104</v>
       </c>
       <c r="G41" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="H41" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="H41" s="24" t="s">
+      <c r="I41" s="24" t="s">
         <v>213</v>
-      </c>
-      <c r="I41" s="24" t="s">
-        <v>214</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>80</v>
@@ -5963,14 +6011,14 @@
         <v>80</v>
       </c>
       <c r="M41" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N41" s="25"/>
       <c r="O41" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="P41" s="34" t="s">
-        <v>215</v>
+      <c r="P41" s="25" t="s">
+        <v>297</v>
       </c>
       <c r="Q41" s="25"/>
       <c r="R41" s="26"/>
@@ -6037,13 +6085,13 @@
         <v>45104</v>
       </c>
       <c r="G43" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="H43" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="I43" s="24" t="s">
         <v>224</v>
-      </c>
-      <c r="H43" s="24" t="s">
-        <v>225</v>
-      </c>
-      <c r="I43" s="24" t="s">
-        <v>226</v>
       </c>
       <c r="J43" s="25" t="s">
         <v>80</v>
@@ -6053,14 +6101,14 @@
         <v>80</v>
       </c>
       <c r="M43" s="25" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="N43" s="25"/>
       <c r="O43" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="P43" s="34" t="s">
-        <v>215</v>
+      <c r="P43" s="25" t="s">
+        <v>298</v>
       </c>
       <c r="Q43" s="25"/>
       <c r="R43" s="26"/>
@@ -6393,13 +6441,13 @@
         <v>45105</v>
       </c>
       <c r="G52" s="33" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H52" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="I52" s="24" t="s">
         <v>234</v>
-      </c>
-      <c r="I52" s="24" t="s">
-        <v>236</v>
       </c>
       <c r="J52" s="25" t="s">
         <v>80</v>
@@ -6437,13 +6485,13 @@
         <v>45104</v>
       </c>
       <c r="G53" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="H53" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="I53" s="24" t="s">
         <v>227</v>
-      </c>
-      <c r="H53" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="I53" s="24" t="s">
-        <v>229</v>
       </c>
       <c r="J53" s="25" t="s">
         <v>80</v>

</xml_diff>